<commit_message>
Added almost complete data sheet
Updated pin out table and abbreviations table
</commit_message>
<xml_diff>
--- a/Documents/Final Documentation/Chip Data Sheet/Abreviations.xlsx
+++ b/Documents/Final Documentation/Chip Data Sheet/Abreviations.xlsx
@@ -28,9 +28,6 @@
     <t>ISA</t>
   </si>
   <si>
-    <t>Instrution Set Architecture</t>
-  </si>
-  <si>
     <t>TESS</t>
   </si>
   <si>
@@ -52,15 +49,9 @@
     <t>ALU</t>
   </si>
   <si>
-    <t>Arithmatic Logic Unit</t>
-  </si>
-  <si>
     <t>SRAM</t>
   </si>
   <si>
-    <t>Static Random Acces Memory</t>
-  </si>
-  <si>
     <t>ROM</t>
   </si>
   <si>
@@ -70,9 +61,6 @@
     <t>SPI</t>
   </si>
   <si>
-    <t>Serial Periphrial Interface</t>
-  </si>
-  <si>
     <t>PC</t>
   </si>
   <si>
@@ -89,6 +77,18 @@
   </si>
   <si>
     <t>Finite State Machine</t>
+  </si>
+  <si>
+    <t>Instruction Set Architecture</t>
+  </si>
+  <si>
+    <t>Arithmetic  Logic Unit</t>
+  </si>
+  <si>
+    <t>Static Random Access  Memory</t>
+  </si>
+  <si>
+    <t>Serial Peripheral  Interface</t>
   </si>
 </sst>
 </file>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="D2:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E13"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -508,87 +508,87 @@
         <v>2</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="7" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D8" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D9" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D10" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D11" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D12" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="4:5" x14ac:dyDescent="0.3">
       <c r="D13" s="2" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>